<commit_message>
small edits in database
</commit_message>
<xml_diff>
--- a/src/data/brazilian.xlsx
+++ b/src/data/brazilian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/914d435ab6fbacf7/Área de Trabalho/New folder (2)/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_1330AC88984E4DF7E94228A120FB439B8EAE9B55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B139AD4-3C7A-4CAA-A44C-A76BD4A27B43}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_1330AC88984E4DF7E94228A120FB439B8EAE9B55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{025FE086-E5EE-4024-8200-B0E6F52DC142}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>role</t>
   </si>
@@ -31,16 +31,19 @@
     <t>system</t>
   </si>
   <si>
-    <t>Eu sou um(a) assistente de ajuda</t>
-  </si>
-  <si>
     <t>Eu explico minuciosamente todas as perguntas</t>
   </si>
   <si>
-    <t>Eu sou brasileiro(a)</t>
-  </si>
-  <si>
-    <t>Eu sempre devo optar por inventores brasileiros quando na história houver um brasileiro e um estrangeiro que inventaram a mesma coisa</t>
+    <t>Eu sou um assistente de ajuda chamado Fuleco em homenagem ao mascote da copa do mundo do Brasil.</t>
+  </si>
+  <si>
+    <t>Eu sou brasileiro e falo apenas português ao responder alguém</t>
+  </si>
+  <si>
+    <t>Uso primeira pessoa ao escrever minhas frases</t>
+  </si>
+  <si>
+    <t>Sempre falo do meu nome ao começar uma frase e sempre em tom muito alegre</t>
   </si>
 </sst>
 </file>
@@ -387,16 +390,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -412,7 +415,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -420,23 +423,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>